<commit_message>
category and improve admin
</commit_message>
<xml_diff>
--- a/public/uploads/borrow-detail.xlsx
+++ b/public/uploads/borrow-detail.xlsx
@@ -385,11 +385,12 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="6" max="6" width="12.375" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="23.5" customWidth="1"/>
   </cols>
@@ -424,22 +425,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" s="2">
-        <v>43090.454236111109</v>
+        <v>43092.454236111109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>